<commit_message>
1a parte da carga, que é carregar a imagem, funcionando. Falta fazer a pipeline e com a pipeline por na tela.
</commit_message>
<xml_diff>
--- a/exdental/tarefas.xlsx
+++ b/exdental/tarefas.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Loader</t>
   </si>
@@ -73,12 +73,15 @@
   </si>
   <si>
     <t>Inverse Radon Transform</t>
+  </si>
+  <si>
+    <t>DOCUMENTAR O QUE FOI FEITO!!!!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,7 +99,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +118,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -128,12 +137,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,7 +417,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -414,151 +425,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G28"/>
+  <dimension ref="A2:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="36.88671875" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="2"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Funcionando o filtro de suavização.
</commit_message>
<xml_diff>
--- a/exdental/tarefas.xlsx
+++ b/exdental/tarefas.xlsx
@@ -143,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -152,6 +152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +425,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -435,7 +436,7 @@
   <dimension ref="A2:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,8 +523,8 @@
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -535,7 +536,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="8" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pela 1a vez o sigmoide no programa
</commit_message>
<xml_diff>
--- a/exdental/tarefas.xlsx
+++ b/exdental/tarefas.xlsx
@@ -143,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -153,6 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,7 +426,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -435,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,8 +548,8 @@
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>